<commit_message>
Test results: 2.280694074 hours / generation
</commit_message>
<xml_diff>
--- a/src/clojush/genesis/test-results/Summary.xlsx
+++ b/src/clojush/genesis/test-results/Summary.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c51537410c5afe56/Projects/Source/Repos/Clojush/src/clojush/genesis/test-results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edgar\OneDrive\Projects\Source\Repos\Clojush\src\clojush\genesis\test-results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{9F68A8CB-F1E4-49AB-9561-8402B1653EEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{E56A84E6-E354-4D94-BF1C-A0015747C0DE}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{9F68A8CB-F1E4-49AB-9561-8402B1653EEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{91477B5E-B770-4B43-A7F0-145C470CAEAF}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" activeTab="1" xr2:uid="{A0E1F8F6-314E-419D-BEFC-0106355C77EA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" activeTab="2" xr2:uid="{A0E1F8F6-314E-419D-BEFC-0106355C77EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Test 1" sheetId="1" r:id="rId1"/>
     <sheet name="Test 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Test 3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -32,12 +33,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>Avg</t>
   </si>
   <si>
     <t>Delta</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -393,7 +397,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -445,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6A4378B-2949-4194-A6BB-7CBA1DE0A0F9}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -505,4 +509,69 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA918793-E908-45CA-AE98-E0701CC37752}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>1537059176163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1537066948183</v>
+      </c>
+      <c r="B2">
+        <f>(A2-A1)/1000/60/60</f>
+        <v>2.1588944444444444</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1537075466130</v>
+      </c>
+      <c r="B3">
+        <f>(A3-A2)/1000/60/60</f>
+        <v>2.3660963888888893</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1537083807659</v>
+      </c>
+      <c r="B4">
+        <f>(A4-A3)/1000/60/60</f>
+        <v>2.3170913888888891</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <f>AVERAGE(B2:B4)</f>
+        <v>2.280694074074074</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1">
+        <f>('Test 2'!B5-'Test 3'!B5)/'Test 1'!B5</f>
+        <v>0.24466025366986752</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Test results: 2.201647037 hours / generation
</commit_message>
<xml_diff>
--- a/src/clojush/genesis/test-results/Summary.xlsx
+++ b/src/clojush/genesis/test-results/Summary.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edgar\OneDrive\Projects\Source\Repos\Clojush\src\clojush\genesis\test-results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{9F68A8CB-F1E4-49AB-9561-8402B1653EEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{91477B5E-B770-4B43-A7F0-145C470CAEAF}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{9F68A8CB-F1E4-49AB-9561-8402B1653EEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{D46EE6F1-1706-480F-9C3F-87FDD19D3739}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" activeTab="2" xr2:uid="{A0E1F8F6-314E-419D-BEFC-0106355C77EA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" activeTab="3" xr2:uid="{A0E1F8F6-314E-419D-BEFC-0106355C77EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Test 1" sheetId="1" r:id="rId1"/>
     <sheet name="Test 2" sheetId="2" r:id="rId2"/>
     <sheet name="Test 3" sheetId="3" r:id="rId3"/>
+    <sheet name="Test 4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>Avg</t>
   </si>
@@ -515,6 +516,71 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA918793-E908-45CA-AE98-E0701CC37752}">
   <dimension ref="A1:B6"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>1537059176163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1537066948183</v>
+      </c>
+      <c r="B2">
+        <f>(A2-A1)/1000/60/60</f>
+        <v>2.1588944444444444</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1537075466130</v>
+      </c>
+      <c r="B3">
+        <f>(A3-A2)/1000/60/60</f>
+        <v>2.3660963888888893</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1537083807659</v>
+      </c>
+      <c r="B4">
+        <f>(A4-A3)/1000/60/60</f>
+        <v>2.3170913888888891</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <f>AVERAGE(B2:B4)</f>
+        <v>2.280694074074074</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1">
+        <f>('Test 2'!B5-'Test 3'!B5)/'Test 2'!B5</f>
+        <v>0.26144912212233035</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF77B1B0-6314-4FA0-8424-58C54921D6C2}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
@@ -523,34 +589,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>1537059176163</v>
+        <v>1537146896653</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1537066948183</v>
+        <v>1537154785973</v>
       </c>
       <c r="B2">
         <f>(A2-A1)/1000/60/60</f>
-        <v>2.1588944444444444</v>
+        <v>2.1914777777777776</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1537075466130</v>
+        <v>1537162973182</v>
       </c>
       <c r="B3">
         <f>(A3-A2)/1000/60/60</f>
-        <v>2.3660963888888893</v>
+        <v>2.2742247222222223</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>1537083807659</v>
+        <v>1537170674441</v>
       </c>
       <c r="B4">
         <f>(A4-A3)/1000/60/60</f>
-        <v>2.3170913888888891</v>
+        <v>2.1392386111111112</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -559,7 +625,7 @@
       </c>
       <c r="B5">
         <f>AVERAGE(B2:B4)</f>
-        <v>2.280694074074074</v>
+        <v>2.2016470370370373</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -567,8 +633,8 @@
         <v>1</v>
       </c>
       <c r="B6" s="1">
-        <f>('Test 2'!B5-'Test 3'!B5)/'Test 1'!B5</f>
-        <v>0.24466025366986752</v>
+        <f>('Test 3'!B5-'Test 4'!B5)/'Test 3'!B5</f>
+        <v>3.4659202185689235E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug fix - Change starting cash from 0 to 10,000.  Configuration - Changed max-generations from 3 to 10.
</commit_message>
<xml_diff>
--- a/src/clojush/genesis/test-results/Summary.xlsx
+++ b/src/clojush/genesis/test-results/Summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edgar\OneDrive\Projects\Source\Repos\Clojush\src\clojush\genesis\test-results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{9F68A8CB-F1E4-49AB-9561-8402B1653EEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{D46EE6F1-1706-480F-9C3F-87FDD19D3739}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="8_{9F68A8CB-F1E4-49AB-9561-8402B1653EEA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{38B7B87E-0025-4AEF-8AEF-2D3BF3044FA1}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" activeTab="3" xr2:uid="{A0E1F8F6-314E-419D-BEFC-0106355C77EA}"/>
   </bookViews>
@@ -579,20 +579,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF77B1B0-6314-4FA0-8424-58C54921D6C2}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1537146896653</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1537154785973</v>
       </c>
@@ -601,7 +601,7 @@
         <v>2.1914777777777776</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1537162973182</v>
       </c>
@@ -610,7 +610,7 @@
         <v>2.2742247222222223</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1537170674441</v>
       </c>
@@ -619,7 +619,7 @@
         <v>2.1392386111111112</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -628,13 +628,19 @@
         <v>2.2016470370370373</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="1">
         <f>('Test 3'!B5-'Test 4'!B5)/'Test 3'!B5</f>
         <v>3.4659202185689235E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <f>24/B5</f>
+        <v>10.900929893058175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>